<commit_message>
Updated the pump inputs
</commit_message>
<xml_diff>
--- a/Inputs/User Inputs 2.xlsx
+++ b/Inputs/User Inputs 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsun/PycharmProjects/Heating-Energy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taraneh\Documents\GitHub\Heating-Energy\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1607347-B577-9647-A50A-C3883DC249AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD5F75D-163C-48F4-ABFF-1DC1AE3BCAE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{EB1BC5F3-6201-40CE-B533-3E2F04EC8AF1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB1BC5F3-6201-40CE-B533-3E2F04EC8AF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="86">
   <si>
     <t xml:space="preserve">Capacity </t>
   </si>
@@ -287,6 +287,21 @@
   </si>
   <si>
     <t>Pump 1</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>hp</t>
+  </si>
+  <si>
+    <t>design or break hoursepower</t>
+  </si>
+  <si>
+    <t>MaxGPM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum pump turn down </t>
   </si>
 </sst>
 </file>
@@ -771,44 +786,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D458F7-2E81-4F85-B480-389326A839C4}">
   <dimension ref="A1:AI34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2" style="10" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="10" width="10.6640625" customWidth="1"/>
-    <col min="11" max="11" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2" style="10" customWidth="1"/>
-    <col min="13" max="13" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" customWidth="1"/>
-    <col min="15" max="16" width="10.6640625" customWidth="1"/>
-    <col min="17" max="17" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" customWidth="1"/>
+    <col min="15" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2" style="10" customWidth="1"/>
-    <col min="19" max="19" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.83203125" customWidth="1"/>
-    <col min="21" max="22" width="10.6640625" customWidth="1"/>
-    <col min="23" max="23" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.85546875" customWidth="1"/>
+    <col min="21" max="22" width="10.7109375" customWidth="1"/>
+    <col min="23" max="23" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="2" style="10" customWidth="1"/>
-    <col min="25" max="25" width="20.83203125" customWidth="1"/>
-    <col min="26" max="27" width="10.6640625" customWidth="1"/>
-    <col min="28" max="28" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.85546875" customWidth="1"/>
+    <col min="26" max="27" width="10.7109375" customWidth="1"/>
+    <col min="28" max="28" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="2" style="10" customWidth="1"/>
-    <col min="30" max="30" width="17.33203125" customWidth="1"/>
-    <col min="31" max="32" width="10.6640625" customWidth="1"/>
+    <col min="30" max="30" width="17.28515625" customWidth="1"/>
+    <col min="31" max="32" width="10.7109375" customWidth="1"/>
     <col min="33" max="33" width="17" customWidth="1"/>
-    <col min="34" max="34" width="39.1640625" customWidth="1"/>
+    <col min="34" max="34" width="39.140625" customWidth="1"/>
     <col min="35" max="35" width="2" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -857,7 +872,7 @@
       <c r="AH1" s="5"/>
       <c r="AI1" s="8"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -950,7 +965,7 @@
       </c>
       <c r="AI2" s="9"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
@@ -1024,7 +1039,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" t="s">
         <v>0</v>
@@ -1049,14 +1064,14 @@
       </c>
       <c r="M4" s="17"/>
       <c r="N4" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="Q4" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="S4" s="17"/>
       <c r="T4" t="s">
@@ -1090,7 +1105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" t="s">
         <v>6</v>
@@ -1115,14 +1130,14 @@
       </c>
       <c r="M5" s="17"/>
       <c r="N5" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="Q5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S5" s="17"/>
       <c r="T5" t="s">
@@ -1146,7 +1161,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" t="s">
         <v>15</v>
@@ -1171,14 +1186,14 @@
       </c>
       <c r="M6" s="17"/>
       <c r="N6" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" t="s">
         <v>14</v>
       </c>
       <c r="Q6" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="S6" s="17"/>
       <c r="T6" t="s">
@@ -1192,7 +1207,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" t="s">
         <v>7</v>
@@ -1217,14 +1232,14 @@
       </c>
       <c r="M7" s="17"/>
       <c r="N7" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="Q7" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="S7" s="17"/>
       <c r="T7" t="s">
@@ -1238,7 +1253,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1271,14 +1286,14 @@
         <v>19</v>
       </c>
       <c r="N8" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" t="s">
         <v>8</v>
       </c>
-      <c r="Q8" s="6" t="s">
-        <v>67</v>
+      <c r="Q8" t="s">
+        <v>8</v>
       </c>
       <c r="R8" s="11"/>
       <c r="S8" t="s">
@@ -1310,7 +1325,17 @@
       </c>
       <c r="AI8" s="11"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" ht="45" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>66</v>
+      </c>
+      <c r="O9" s="1"/>
+      <c r="P9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="AD9" t="s">
         <v>53</v>
       </c>
@@ -1318,7 +1343,7 @@
       <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="AD10" t="s">
         <v>49</v>
       </c>
@@ -1326,7 +1351,7 @@
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
@@ -1352,19 +1377,6 @@
       </c>
       <c r="K11" s="13" t="s">
         <v>17</v>
-      </c>
-      <c r="M11" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="N11" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="O11" s="14"/>
-      <c r="P11" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q11" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="S11" s="16" t="s">
         <v>79</v>
@@ -1386,7 +1398,7 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="7" t="s">
         <v>0</v>
@@ -1409,16 +1421,18 @@
       <c r="K12" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="M12" s="17"/>
-      <c r="N12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O12" s="12"/>
-      <c r="P12" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q12" s="7" t="s">
-        <v>11</v>
+      <c r="M12" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="O12" s="14"/>
+      <c r="P12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q12" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="S12" s="17"/>
       <c r="T12" t="s">
@@ -1438,7 +1452,7 @@
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="7" t="s">
         <v>6</v>
@@ -1463,14 +1477,14 @@
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="7" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O13" s="12"/>
       <c r="P13" s="7" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S13" s="17"/>
       <c r="T13" t="s">
@@ -1490,7 +1504,7 @@
       <c r="AF13" s="1"/>
       <c r="AG13" s="1"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="7" t="s">
         <v>15</v>
@@ -1515,14 +1529,14 @@
       </c>
       <c r="M14" s="17"/>
       <c r="N14" s="7" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="O14" s="12"/>
       <c r="P14" s="7" t="s">
         <v>14</v>
       </c>
       <c r="Q14" s="7" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="S14" s="17"/>
       <c r="T14" t="s">
@@ -1536,7 +1550,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="7" t="s">
         <v>7</v>
@@ -1561,14 +1575,14 @@
       </c>
       <c r="M15" s="17"/>
       <c r="N15" s="7" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="O15" s="12"/>
       <c r="P15" s="7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="Q15" s="7" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="S15" s="17"/>
       <c r="T15" t="s">
@@ -1582,7 +1596,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>19</v>
       </c>
@@ -1611,18 +1625,16 @@
         <v>21</v>
       </c>
       <c r="L16" s="11"/>
-      <c r="M16" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="M16" s="17"/>
       <c r="N16" s="7" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="O16" s="12"/>
       <c r="P16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Q16" s="15" t="s">
-        <v>67</v>
+      <c r="Q16" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="R16" s="11"/>
       <c r="S16" t="s">
@@ -1654,7 +1666,20 @@
       </c>
       <c r="AI16" s="11"/>
     </row>
-    <row r="17" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="17" spans="7:33" ht="45" x14ac:dyDescent="0.25">
+      <c r="M17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="O17" s="12"/>
+      <c r="P17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q17" s="15" t="s">
+        <v>67</v>
+      </c>
       <c r="AD17" t="s">
         <v>48</v>
       </c>
@@ -1662,7 +1687,7 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
     </row>
-    <row r="18" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:33" x14ac:dyDescent="0.25">
       <c r="AD18" t="s">
         <v>53</v>
       </c>
@@ -1670,7 +1695,7 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
     </row>
-    <row r="19" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G19" t="s">
         <v>25</v>
       </c>
@@ -1690,7 +1715,7 @@
       <c r="AF19" s="1"/>
       <c r="AG19" s="1"/>
     </row>
-    <row r="20" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="20" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1702,7 +1727,7 @@
       <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
     </row>
-    <row r="21" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="21" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1714,7 +1739,7 @@
       <c r="AF21" s="1"/>
       <c r="AG21" s="1"/>
     </row>
-    <row r="22" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="22" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1726,73 +1751,73 @@
       <c r="AF22" s="1"/>
       <c r="AG22" s="1"/>
     </row>
-    <row r="23" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="23" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="25" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="26" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="27" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="28" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="29" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="30" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="31" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="7:33" x14ac:dyDescent="0.2">
+    <row r="32" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -1801,7 +1826,7 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="G11:G15"/>
-    <mergeCell ref="M11:M15"/>
+    <mergeCell ref="M12:M16"/>
     <mergeCell ref="S3:S7"/>
     <mergeCell ref="S11:S15"/>
     <mergeCell ref="A3:A7"/>
@@ -1822,13 +1847,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>23</v>
       </c>
@@ -1836,7 +1861,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1845,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1854,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1863,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1872,7 +1897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1881,7 +1906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1903,12 +1928,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>29</v>
       </c>
@@ -1916,27 +1941,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1954,9 +1979,9 @@
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>80</v>
       </c>
@@ -1964,27 +1989,27 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -2002,12 +2027,12 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>78</v>
       </c>
@@ -2015,27 +2040,27 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2053,7 +2078,7 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2065,7 +2090,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 'Time' column to EquipmentOutput dataframe.
</commit_message>
<xml_diff>
--- a/Inputs/User Inputs 2.xlsx
+++ b/Inputs/User Inputs 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taraneh\Documents\GitHub\Heating-Energy\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Herrera\Documents\My Documents\My Training\Python\Scripts\Heating-Energy\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD5F75D-163C-48F4-ABFF-1DC1AE3BCAE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE5C8B0-F49B-4CE1-B02C-9DE7B106DE84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB1BC5F3-6201-40CE-B533-3E2F04EC8AF1}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{EB1BC5F3-6201-40CE-B533-3E2F04EC8AF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -431,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
@@ -469,6 +468,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -786,44 +786,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D458F7-2E81-4F85-B480-389326A839C4}">
   <dimension ref="A1:AI34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AE28" sqref="AE28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2" style="10" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" customWidth="1"/>
+    <col min="9" max="10" width="10.6640625" customWidth="1"/>
+    <col min="11" max="11" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2" style="10" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" customWidth="1"/>
-    <col min="15" max="16" width="10.7109375" customWidth="1"/>
-    <col min="17" max="17" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.88671875" customWidth="1"/>
+    <col min="15" max="16" width="10.6640625" customWidth="1"/>
+    <col min="17" max="17" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2" style="10" customWidth="1"/>
-    <col min="19" max="19" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.85546875" customWidth="1"/>
-    <col min="21" max="22" width="10.7109375" customWidth="1"/>
-    <col min="23" max="23" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.88671875" customWidth="1"/>
+    <col min="21" max="22" width="10.6640625" customWidth="1"/>
+    <col min="23" max="23" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="2" style="10" customWidth="1"/>
-    <col min="25" max="25" width="20.85546875" customWidth="1"/>
-    <col min="26" max="27" width="10.7109375" customWidth="1"/>
-    <col min="28" max="28" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.88671875" customWidth="1"/>
+    <col min="26" max="27" width="10.6640625" customWidth="1"/>
+    <col min="28" max="28" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="2" style="10" customWidth="1"/>
-    <col min="30" max="30" width="17.28515625" customWidth="1"/>
-    <col min="31" max="32" width="10.7109375" customWidth="1"/>
+    <col min="30" max="30" width="17.33203125" customWidth="1"/>
+    <col min="31" max="32" width="10.6640625" customWidth="1"/>
     <col min="33" max="33" width="17" customWidth="1"/>
-    <col min="34" max="34" width="39.140625" customWidth="1"/>
+    <col min="34" max="34" width="39.109375" customWidth="1"/>
     <col min="35" max="35" width="2" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -872,7 +872,7 @@
       <c r="AH1" s="5"/>
       <c r="AI1" s="8"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -965,7 +965,7 @@
       </c>
       <c r="AI2" s="9"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" t="s">
         <v>0</v>
@@ -1105,7 +1105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
       <c r="B5" t="s">
         <v>6</v>
@@ -1161,7 +1161,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" t="s">
         <v>15</v>
@@ -1207,7 +1207,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" t="s">
         <v>7</v>
@@ -1253,7 +1253,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="AI8" s="11"/>
     </row>
-    <row r="9" spans="1:35" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="43.2" x14ac:dyDescent="0.3">
       <c r="N9" t="s">
         <v>66</v>
       </c>
@@ -1339,19 +1339,31 @@
       <c r="AD9" t="s">
         <v>53</v>
       </c>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AE9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AD10" t="s">
         <v>49</v>
       </c>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AE10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>8</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
@@ -1394,11 +1406,17 @@
       <c r="AD11" t="s">
         <v>50</v>
       </c>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1"/>
-      <c r="AG11" s="1"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AE11" s="1">
+        <v>9</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>12</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="7" t="s">
         <v>0</v>
@@ -1448,11 +1466,17 @@
       <c r="AD12" t="s">
         <v>51</v>
       </c>
-      <c r="AE12" s="1"/>
-      <c r="AF12" s="1"/>
-      <c r="AG12" s="1"/>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AE12" s="1">
+        <v>13</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>18</v>
+      </c>
+      <c r="AG12" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="7" t="s">
         <v>6</v>
@@ -1500,11 +1524,17 @@
       <c r="AD13" t="s">
         <v>52</v>
       </c>
-      <c r="AE13" s="1"/>
-      <c r="AF13" s="1"/>
-      <c r="AG13" s="1"/>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AE13" s="1">
+        <v>19</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>24</v>
+      </c>
+      <c r="AG13" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="7" t="s">
         <v>15</v>
@@ -1550,7 +1580,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="7" t="s">
         <v>7</v>
@@ -1596,7 +1626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>19</v>
       </c>
@@ -1666,7 +1696,7 @@
       </c>
       <c r="AI16" s="11"/>
     </row>
-    <row r="17" spans="7:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:33" ht="43.2" x14ac:dyDescent="0.3">
       <c r="M17" s="7" t="s">
         <v>19</v>
       </c>
@@ -1683,19 +1713,31 @@
       <c r="AD17" t="s">
         <v>48</v>
       </c>
-      <c r="AE17" s="1"/>
-      <c r="AF17" s="1"/>
-      <c r="AG17" s="1"/>
-    </row>
-    <row r="18" spans="7:33" x14ac:dyDescent="0.25">
+      <c r="AE17" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG17" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="18" spans="7:33" x14ac:dyDescent="0.3">
       <c r="AD18" t="s">
         <v>53</v>
       </c>
-      <c r="AE18" s="1"/>
-      <c r="AF18" s="1"/>
-      <c r="AG18" s="1"/>
-    </row>
-    <row r="19" spans="7:33" x14ac:dyDescent="0.25">
+      <c r="AE18" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF18" s="1">
+        <v>8</v>
+      </c>
+      <c r="AG18" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="19" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G19" t="s">
         <v>25</v>
       </c>
@@ -1711,11 +1753,17 @@
       <c r="AD19" t="s">
         <v>49</v>
       </c>
-      <c r="AE19" s="1"/>
-      <c r="AF19" s="1"/>
-      <c r="AG19" s="1"/>
-    </row>
-    <row r="20" spans="7:33" x14ac:dyDescent="0.25">
+      <c r="AE19" s="1">
+        <v>9</v>
+      </c>
+      <c r="AF19" s="1">
+        <v>12</v>
+      </c>
+      <c r="AG19" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="20" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1723,11 +1771,17 @@
       <c r="AD20" t="s">
         <v>50</v>
       </c>
-      <c r="AE20" s="1"/>
-      <c r="AF20" s="1"/>
-      <c r="AG20" s="1"/>
-    </row>
-    <row r="21" spans="7:33" x14ac:dyDescent="0.25">
+      <c r="AE20" s="1">
+        <v>13</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>18</v>
+      </c>
+      <c r="AG20" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="21" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1735,11 +1789,17 @@
       <c r="AD21" t="s">
         <v>51</v>
       </c>
-      <c r="AE21" s="1"/>
-      <c r="AF21" s="1"/>
-      <c r="AG21" s="1"/>
-    </row>
-    <row r="22" spans="7:33" x14ac:dyDescent="0.25">
+      <c r="AE21" s="1">
+        <v>19</v>
+      </c>
+      <c r="AF21" s="1">
+        <v>22</v>
+      </c>
+      <c r="AG21" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="22" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1747,77 +1807,89 @@
       <c r="AD22" t="s">
         <v>52</v>
       </c>
-      <c r="AE22" s="1"/>
-      <c r="AF22" s="1"/>
-      <c r="AG22" s="1"/>
-    </row>
-    <row r="23" spans="7:33" x14ac:dyDescent="0.25">
+      <c r="AE22" s="1">
+        <v>23</v>
+      </c>
+      <c r="AF22" s="1">
+        <v>24</v>
+      </c>
+      <c r="AG22" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="23" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="7:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="7:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="7:33" x14ac:dyDescent="0.25">
+      <c r="AE25" s="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="7:33" x14ac:dyDescent="0.25">
+      <c r="AE26" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="7:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="7:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="7:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="7:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="7:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:33" x14ac:dyDescent="0.3">
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -1847,13 +1919,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>23</v>
       </c>
@@ -1861,7 +1933,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1870,7 +1942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1879,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1888,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1897,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1906,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1928,12 +2000,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>29</v>
       </c>
@@ -1941,27 +2013,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1979,9 +2051,9 @@
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>80</v>
       </c>
@@ -1989,27 +2061,27 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -2027,12 +2099,12 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>78</v>
       </c>
@@ -2040,27 +2112,27 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2078,7 +2150,7 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2090,7 +2162,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>